<commit_message>
wording for bugs fixed
</commit_message>
<xml_diff>
--- a/release-notes/2024-12/closed-bugs-sle-2024-12.xlsx
+++ b/release-notes/2024-12/closed-bugs-sle-2024-12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emerson.sharepoint.com/sites/TM-IoTProgram/Shared Documents/ProjectDocuments/SystemLink 2024/2025 Q1 (v.25.0)(releasing out of Cycle 24.C4)/Common docs/Release Notes/SLE 2024-12 Release Notes - December/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/install-systemlink-enterprise/release-notes/2024-12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{0357FC32-4DB0-FA47-B55E-60093BEFF741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01434302-3E41-4E71-8979-DC44B90768A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528CCB85-3105-4443-B8A8-BEBA31CA4F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19320" yWindow="500" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="closed bugs in last iteration" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Location movement stuck if you make 2 consecutive move to the same system</t>
   </si>
   <si>
-    <t>Loading mask glitch when deleting more packages in Packages grid from Feed details</t>
-  </si>
-  <si>
     <t>Custom properties on assets not being saved</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Updating notebook in jupyter is not getting reflected in dataspace analysis</t>
   </si>
   <si>
-    <t>Security vulnerabilities in ni-grafana</t>
-  </si>
-  <si>
     <t>Column headers are not localized on the routines grid</t>
   </si>
   <si>
@@ -93,6 +87,12 @@
   </si>
   <si>
     <t>Update work order details page to auto refresh</t>
+  </si>
+  <si>
+    <t>Loading mask artifacat when deleting packages in Packages grid from Feed details</t>
+  </si>
+  <si>
+    <t>Update Grafana dependencies to resolve public CVEs</t>
   </si>
 </sst>
 </file>
@@ -947,15 +947,15 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="110.375" customWidth="1"/>
+    <col min="2" max="2" width="110.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -966,7 +966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2924664</v>
       </c>
@@ -977,7 +977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2924670</v>
       </c>
@@ -988,7 +988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2929060</v>
       </c>
@@ -999,215 +999,215 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2929769</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2931424</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>2936711</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>2928870</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2929028</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>2938987</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>2939368</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>2901954</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>2912051</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>2929271</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>2929230</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2924964</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
     </row>
@@ -1220,6 +1220,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8f35f8fb-94b8-4296-88b5-253c68a5f93d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC68938C25E75A48B38E3943F7278D4C" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d58f385c17140d35cbd71f1f19d1bc6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9" xmlns:ns3="8f35f8fb-94b8-4296-88b5-253c68a5f93d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6fea239938238ce97a7c0b11cdae990" ns2:_="" ns3:_="">
     <xsd:import namespace="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
@@ -1468,17 +1479,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8f35f8fb-94b8-4296-88b5-253c68a5f93d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1489,6 +1489,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
+    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD13E7E-916C-4710-89E9-937C762EA783}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1507,23 +1524,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
-    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
SLE 2024-12 Closed Bugs update to include 2935004
2935004: Fix ServiceRegistry not being able to communicate with JupyterHub when a CNI with NetworkPolicy support is installed
</commit_message>
<xml_diff>
--- a/release-notes/2024-12/closed-bugs-sle-2024-12.xlsx
+++ b/release-notes/2024-12/closed-bugs-sle-2024-12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/install-systemlink-enterprise/release-notes/2024-12/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emerson.sharepoint.com/sites/TM-IoTProgram/Shared Documents/ProjectDocuments/SystemLink 2024/2025 Q1 (v.25.0)(releasing out of Cycle 24.C4)/Common docs/Release Notes/SLE 2024-12 Release Notes - December/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528CCB85-3105-4443-B8A8-BEBA31CA4F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5939EF5-9311-4F82-8B86-74ECEE5719CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19320" yWindow="500" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="closed bugs in last iteration" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -47,18 +47,21 @@
     <t>State</t>
   </si>
   <si>
+    <t xml:space="preserve">Datepicker from query location does not work after calibration date picker was used </t>
+  </si>
+  <si>
     <t>Closed</t>
   </si>
   <si>
-    <t xml:space="preserve">Datepicker from query location does not work after calibration date picker was used </t>
-  </si>
-  <si>
     <t>Datepicker from query location does not work after upload files slideout was open</t>
   </si>
   <si>
     <t>Location movement stuck if you make 2 consecutive move to the same system</t>
   </si>
   <si>
+    <t>Loading mask glitch when deleting more packages in Packages grid from Feed details</t>
+  </si>
+  <si>
     <t>Custom properties on assets not being saved</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
     <t>Updating notebook in jupyter is not getting reflected in dataspace analysis</t>
   </si>
   <si>
+    <t>Security vulnerabilities in ni-grafana</t>
+  </si>
+  <si>
     <t>Column headers are not localized on the routines grid</t>
   </si>
   <si>
@@ -89,17 +95,14 @@
     <t>Update work order details page to auto refresh</t>
   </si>
   <si>
-    <t>Loading mask artifacat when deleting packages in Packages grid from Feed details</t>
-  </si>
-  <si>
-    <t>Update Grafana dependencies to resolve public CVEs</t>
+    <t>Fix ServiceRegistry not being able to communicate with JupyterHub when a CNI with NetworkPolicy support is installed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -648,9 +651,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -688,7 +691,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -794,7 +797,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -936,7 +939,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -947,15 +950,15 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="110.33203125" customWidth="1"/>
+    <col min="2" max="2" width="110.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -966,18 +969,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="3">
         <v>2924664</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="3">
         <v>2924670</v>
       </c>
@@ -985,10 +988,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="3">
         <v>2929060</v>
       </c>
@@ -996,218 +999,225 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="3">
         <v>2929769</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="3">
         <v>2931424</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="3">
         <v>2936711</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="3">
         <v>2928870</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="A9" s="3">
         <v>2929028</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="A10" s="3">
         <v>2938987</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="3">
         <v>2939368</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="3">
         <v>2901954</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="3">
         <v>2912051</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="3">
         <v>2929271</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="3">
         <v>2929230</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="3">
         <v>2924964</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A17" s="3">
+        <v>2935004</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
     </row>
@@ -1489,45 +1499,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
-    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD13E7E-916C-4710-89E9-937C762EA783}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
-    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD13E7E-916C-4710-89E9-937C762EA783}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}"/>
 </file>
</xml_diff>

<commit_message>
SLE 2024-12 Closed Bugs update to include 2935004 (#241)
* SLE 2024-12 Closed Bugs update to include 2935004

2935004: Fix ServiceRegistry not being able to communicate with JupyterHub when a CNI with NetworkPolicy support is installed

* updated bug text

---------

Co-authored-by: Mark Black <mark.black@emerson.com>
</commit_message>
<xml_diff>
--- a/release-notes/2024-12/closed-bugs-sle-2024-12.xlsx
+++ b/release-notes/2024-12/closed-bugs-sle-2024-12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/install-systemlink-enterprise/release-notes/2024-12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528CCB85-3105-4443-B8A8-BEBA31CA4F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9216204A-B12F-8B43-BE55-945C56575686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19320" yWindow="500" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="closed bugs in last iteration" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -47,18 +47,21 @@
     <t>State</t>
   </si>
   <si>
+    <t xml:space="preserve">Datepicker from query location does not work after calibration date picker was used </t>
+  </si>
+  <si>
     <t>Closed</t>
   </si>
   <si>
-    <t xml:space="preserve">Datepicker from query location does not work after calibration date picker was used </t>
-  </si>
-  <si>
     <t>Datepicker from query location does not work after upload files slideout was open</t>
   </si>
   <si>
     <t>Location movement stuck if you make 2 consecutive move to the same system</t>
   </si>
   <si>
+    <t>Loading mask glitch when deleting more packages in Packages grid from Feed details</t>
+  </si>
+  <si>
     <t>Custom properties on assets not being saved</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
     <t>Updating notebook in jupyter is not getting reflected in dataspace analysis</t>
   </si>
   <si>
+    <t>Security vulnerabilities in ni-grafana</t>
+  </si>
+  <si>
     <t>Column headers are not localized on the routines grid</t>
   </si>
   <si>
@@ -89,10 +95,7 @@
     <t>Update work order details page to auto refresh</t>
   </si>
   <si>
-    <t>Loading mask artifacat when deleting packages in Packages grid from Feed details</t>
-  </si>
-  <si>
-    <t>Update Grafana dependencies to resolve public CVEs</t>
+    <t>Scripts (JupyterHub) not shown in navigation tree when a CNI with NetworkPolicy support is installed</t>
   </si>
 </sst>
 </file>
@@ -947,7 +950,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -971,10 +974,10 @@
         <v>2924664</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,7 +988,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -996,7 +999,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1004,10 +1007,10 @@
         <v>2929769</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1015,10 +1018,10 @@
         <v>2931424</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1026,10 +1029,10 @@
         <v>2936711</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1037,10 +1040,10 @@
         <v>2928870</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1048,10 +1051,10 @@
         <v>2929028</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1059,10 +1062,10 @@
         <v>2938987</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1070,10 +1073,10 @@
         <v>2939368</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,10 +1084,10 @@
         <v>2901954</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1092,10 +1095,10 @@
         <v>2912051</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1103,10 +1106,10 @@
         <v>2929271</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1114,10 +1117,10 @@
         <v>2929230</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1125,73 +1128,80 @@
         <v>2924964</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>2935004</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
@@ -1220,17 +1230,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8f35f8fb-94b8-4296-88b5-253c68a5f93d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC68938C25E75A48B38E3943F7278D4C" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d58f385c17140d35cbd71f1f19d1bc6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9" xmlns:ns3="8f35f8fb-94b8-4296-88b5-253c68a5f93d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6fea239938238ce97a7c0b11cdae990" ns2:_="" ns3:_="">
     <xsd:import namespace="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
@@ -1479,6 +1478,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8f35f8fb-94b8-4296-88b5-253c68a5f93d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1489,23 +1499,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
-    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDD13E7E-916C-4710-89E9-937C762EA783}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1524,6 +1517,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6B2099-BF96-40FC-B6D0-611F0B5B8DEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="58dd0d8a-0b6e-4df8-afdb-fbe9bd3e42e9"/>
+    <ds:schemaRef ds:uri="8f35f8fb-94b8-4296-88b5-253c68a5f93d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F5BA7BF-C649-45A8-BA98-72C6A48D6AFB}">
   <ds:schemaRefs>

</xml_diff>